<commit_message>
updated cw for climate watch data
</commit_message>
<xml_diff>
--- a/ref/data_crosswalks/sisepuede_fields_to_climate_watch_emissions_map.xlsx
+++ b/ref/data_crosswalks/sisepuede_fields_to_climate_watch_emissions_map.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jsyme/Documents/Projects/git_jbus/lac_decarbonization/ref/data_crosswalks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95E213E0-38E4-C844-928D-7B3532ED7D59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{954A7B27-3176-3A48-B825-88654719A002}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="620" yWindow="500" windowWidth="24420" windowHeight="17440" xr2:uid="{155FF7EE-733C-FD4A-B2A0-931C190B7245}"/>
+    <workbookView xWindow="180" yWindow="500" windowWidth="21840" windowHeight="20400" xr2:uid="{155FF7EE-733C-FD4A-B2A0-931C190B7245}"/>
   </bookViews>
   <sheets>
     <sheet name="climate_watch_emissions" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="183">
   <si>
     <t>gas</t>
   </si>
@@ -582,6 +582,9 @@
   </si>
   <si>
     <t>Fields available in SISEPUEDE, but purposefully excluded to match CW Method</t>
+  </si>
+  <si>
+    <t>include</t>
   </si>
 </sst>
 </file>
@@ -1036,7 +1039,7 @@
   <dimension ref="A1:G160"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1060,6 +1063,9 @@
       <c r="D1" s="8" t="s">
         <v>32</v>
       </c>
+      <c r="E1" s="8" t="s">
+        <v>182</v>
+      </c>
       <c r="F1" t="s">
         <v>179</v>
       </c>
@@ -1080,6 +1086,9 @@
       <c r="D2" s="2" t="s">
         <v>66</v>
       </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -1095,6 +1104,9 @@
       <c r="D3" s="2" t="s">
         <v>68</v>
       </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
       <c r="F3" s="5" t="s">
         <v>5</v>
       </c>
@@ -1112,6 +1124,9 @@
       <c r="D4" s="2" t="s">
         <v>122</v>
       </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
       <c r="F4" s="6" t="s">
         <v>180</v>
       </c>
@@ -1129,6 +1144,9 @@
       <c r="D5" s="2" t="s">
         <v>124</v>
       </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
       <c r="F5" s="7" t="s">
         <v>181</v>
       </c>
@@ -1146,6 +1164,9 @@
       <c r="D6" s="2" t="s">
         <v>175</v>
       </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -1160,6 +1181,9 @@
       <c r="D7" s="2" t="s">
         <v>177</v>
       </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
@@ -1174,6 +1198,9 @@
       <c r="D8" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
@@ -1188,6 +1215,9 @@
       <c r="D9" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
@@ -1202,6 +1232,9 @@
       <c r="D10" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
@@ -1216,6 +1249,9 @@
       <c r="D11" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
@@ -1230,6 +1266,9 @@
       <c r="D12" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
@@ -1244,6 +1283,9 @@
       <c r="D13" s="3" t="s">
         <v>10</v>
       </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
@@ -1258,6 +1300,9 @@
       <c r="D14" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
@@ -1272,6 +1317,9 @@
       <c r="D15" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
@@ -1286,8 +1334,11 @@
       <c r="D16" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -1300,8 +1351,11 @@
       <c r="D17" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -1314,8 +1368,11 @@
       <c r="D18" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>34</v>
       </c>
@@ -1328,8 +1385,11 @@
       <c r="D19" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>34</v>
       </c>
@@ -1342,8 +1402,11 @@
       <c r="D20" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>34</v>
       </c>
@@ -1356,8 +1419,11 @@
       <c r="D21" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>34</v>
       </c>
@@ -1370,8 +1436,11 @@
       <c r="D22" s="3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>34</v>
       </c>
@@ -1384,8 +1453,11 @@
       <c r="D23" s="3" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>34</v>
       </c>
@@ -1398,8 +1470,11 @@
       <c r="D24" s="3" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>34</v>
       </c>
@@ -1412,8 +1487,11 @@
       <c r="D25" s="3" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>34</v>
       </c>
@@ -1426,8 +1504,11 @@
       <c r="D26" s="2" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>34</v>
       </c>
@@ -1440,8 +1521,11 @@
       <c r="D27" s="2" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>34</v>
       </c>
@@ -1454,8 +1538,11 @@
       <c r="D28" s="2" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>34</v>
       </c>
@@ -1468,8 +1555,11 @@
       <c r="D29" s="3" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>34</v>
       </c>
@@ -1482,8 +1572,11 @@
       <c r="D30" s="2" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>34</v>
       </c>
@@ -1496,8 +1589,11 @@
       <c r="D31" s="3" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>34</v>
       </c>
@@ -1510,8 +1606,11 @@
       <c r="D32" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>34</v>
       </c>
@@ -1524,8 +1623,11 @@
       <c r="D33" s="2" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>34</v>
       </c>
@@ -1538,8 +1640,11 @@
       <c r="D34" s="2" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -1552,8 +1657,11 @@
       <c r="D35" s="2" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>34</v>
       </c>
@@ -1566,8 +1674,11 @@
       <c r="D36" s="2" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>34</v>
       </c>
@@ -1580,8 +1691,11 @@
       <c r="D37" s="2" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>34</v>
       </c>
@@ -1594,8 +1708,11 @@
       <c r="D38" s="2" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>34</v>
       </c>
@@ -1608,8 +1725,11 @@
       <c r="D39" s="2" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>34</v>
       </c>
@@ -1622,8 +1742,11 @@
       <c r="D40" s="3" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>34</v>
       </c>
@@ -1636,8 +1759,11 @@
       <c r="D41" s="3" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>34</v>
       </c>
@@ -1650,8 +1776,11 @@
       <c r="D42" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>34</v>
       </c>
@@ -1664,8 +1793,11 @@
       <c r="D43" s="3" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>34</v>
       </c>
@@ -1678,8 +1810,11 @@
       <c r="D44" s="2" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>34</v>
       </c>
@@ -1692,8 +1827,11 @@
       <c r="D45" s="2" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>34</v>
       </c>
@@ -1706,8 +1844,11 @@
       <c r="D46" s="2" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>34</v>
       </c>
@@ -1720,8 +1861,11 @@
       <c r="D47" s="3" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>34</v>
       </c>
@@ -1734,8 +1878,11 @@
       <c r="D48" s="2" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>34</v>
       </c>
@@ -1748,8 +1895,11 @@
       <c r="D49" s="3" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>34</v>
       </c>
@@ -1762,8 +1912,11 @@
       <c r="D50" s="2" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>34</v>
       </c>
@@ -1776,8 +1929,11 @@
       <c r="D51" s="2" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>34</v>
       </c>
@@ -1790,8 +1946,11 @@
       <c r="D52" s="2" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>34</v>
       </c>
@@ -1804,8 +1963,11 @@
       <c r="D53" s="2" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>34</v>
       </c>
@@ -1818,8 +1980,11 @@
       <c r="D54" s="2" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>34</v>
       </c>
@@ -1832,8 +1997,11 @@
       <c r="D55" s="2" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>34</v>
       </c>
@@ -1846,8 +2014,11 @@
       <c r="D56" s="2" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>34</v>
       </c>
@@ -1860,8 +2031,11 @@
       <c r="D57" s="2" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>34</v>
       </c>
@@ -1874,8 +2048,11 @@
       <c r="D58" s="3" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>34</v>
       </c>
@@ -1888,8 +2065,11 @@
       <c r="D59" s="3" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>34</v>
       </c>
@@ -1902,8 +2082,11 @@
       <c r="D60" s="3" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>34</v>
       </c>
@@ -1916,8 +2099,11 @@
       <c r="D61" s="3" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>39</v>
       </c>
@@ -1930,8 +2116,11 @@
       <c r="D62" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>39</v>
       </c>
@@ -1944,8 +2133,11 @@
       <c r="D63" s="2" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>39</v>
       </c>
@@ -1958,8 +2150,11 @@
       <c r="D64" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" s="9" t="s">
         <v>39</v>
       </c>
@@ -1972,8 +2167,11 @@
       <c r="D65" s="4" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>39</v>
       </c>
@@ -1986,8 +2184,11 @@
       <c r="D66" s="2" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>39</v>
       </c>
@@ -2000,8 +2201,11 @@
       <c r="D67" s="2" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E67">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" s="9" t="s">
         <v>39</v>
       </c>
@@ -2014,8 +2218,11 @@
       <c r="D68" s="4" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" s="9" t="s">
         <v>39</v>
       </c>
@@ -2028,8 +2235,11 @@
       <c r="D69" s="4" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" s="9" t="s">
         <v>39</v>
       </c>
@@ -2042,8 +2252,11 @@
       <c r="D70" s="4" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>44</v>
       </c>
@@ -2056,8 +2269,11 @@
       <c r="D71" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>44</v>
       </c>
@@ -2070,8 +2286,11 @@
       <c r="D72" s="2" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E72">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>44</v>
       </c>
@@ -2084,8 +2303,11 @@
       <c r="D73" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>44</v>
       </c>
@@ -2098,8 +2320,11 @@
       <c r="D74" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>44</v>
       </c>
@@ -2112,8 +2337,11 @@
       <c r="D75" s="2" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>44</v>
       </c>
@@ -2126,8 +2354,11 @@
       <c r="D76" s="2" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>44</v>
       </c>
@@ -2140,8 +2371,11 @@
       <c r="D77" s="2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>44</v>
       </c>
@@ -2154,8 +2388,11 @@
       <c r="D78" s="2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>44</v>
       </c>
@@ -2168,8 +2405,11 @@
       <c r="D79" s="2" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E79">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>44</v>
       </c>
@@ -2182,8 +2422,11 @@
       <c r="D80" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>44</v>
       </c>
@@ -2196,8 +2439,11 @@
       <c r="D81" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E81">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>44</v>
       </c>
@@ -2210,8 +2456,11 @@
       <c r="D82" s="2" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E82">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>44</v>
       </c>
@@ -2224,8 +2473,11 @@
       <c r="D83" s="2" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>44</v>
       </c>
@@ -2238,8 +2490,11 @@
       <c r="D84" s="2" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>44</v>
       </c>
@@ -2252,8 +2507,11 @@
       <c r="D85" s="2" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E85">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>44</v>
       </c>
@@ -2266,8 +2524,11 @@
       <c r="D86" s="2" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>44</v>
       </c>
@@ -2280,8 +2541,11 @@
       <c r="D87" s="2" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E87">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>44</v>
       </c>
@@ -2294,8 +2558,11 @@
       <c r="D88" s="2" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>44</v>
       </c>
@@ -2308,8 +2575,11 @@
       <c r="D89" s="2" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E89">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>44</v>
       </c>
@@ -2322,8 +2592,11 @@
       <c r="D90" s="2" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E90">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>44</v>
       </c>
@@ -2336,8 +2609,11 @@
       <c r="D91" s="2" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E91">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>44</v>
       </c>
@@ -2350,8 +2626,11 @@
       <c r="D92" s="2" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E92">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>44</v>
       </c>
@@ -2364,8 +2643,11 @@
       <c r="D93" s="2" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E93">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>44</v>
       </c>
@@ -2378,8 +2660,11 @@
       <c r="D94" s="2" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E94">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>44</v>
       </c>
@@ -2392,8 +2677,11 @@
       <c r="D95" s="2" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E95">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>44</v>
       </c>
@@ -2406,8 +2694,11 @@
       <c r="D96" s="2" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>44</v>
       </c>
@@ -2420,8 +2711,11 @@
       <c r="D97" s="2" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>44</v>
       </c>
@@ -2434,8 +2728,11 @@
       <c r="D98" s="2" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E98">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>44</v>
       </c>
@@ -2448,8 +2745,11 @@
       <c r="D99" s="2" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>44</v>
       </c>
@@ -2462,8 +2762,11 @@
       <c r="D100" s="2" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E100">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>44</v>
       </c>
@@ -2476,8 +2779,11 @@
       <c r="D101" s="2" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>44</v>
       </c>
@@ -2490,8 +2796,11 @@
       <c r="D102" s="2" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E102">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>44</v>
       </c>
@@ -2504,8 +2813,11 @@
       <c r="D103" s="2" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E103">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>44</v>
       </c>
@@ -2518,8 +2830,11 @@
       <c r="D104" s="2" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E104">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>44</v>
       </c>
@@ -2532,8 +2847,11 @@
       <c r="D105" s="2" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E105">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>44</v>
       </c>
@@ -2546,8 +2864,11 @@
       <c r="D106" s="2" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E106">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>44</v>
       </c>
@@ -2560,8 +2881,11 @@
       <c r="D107" s="2" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E107">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>44</v>
       </c>
@@ -2574,8 +2898,11 @@
       <c r="D108" s="2" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E108">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>44</v>
       </c>
@@ -2588,8 +2915,11 @@
       <c r="D109" s="2" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E109">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>44</v>
       </c>
@@ -2602,8 +2932,11 @@
       <c r="D110" s="2" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E110">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>44</v>
       </c>
@@ -2616,8 +2949,11 @@
       <c r="D111" s="2" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E111">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>44</v>
       </c>
@@ -2630,8 +2966,11 @@
       <c r="D112" s="2" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E112">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>44</v>
       </c>
@@ -2644,8 +2983,11 @@
       <c r="D113" s="2" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E113">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>44</v>
       </c>
@@ -2658,8 +3000,11 @@
       <c r="D114" s="2" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E114">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>44</v>
       </c>
@@ -2672,8 +3017,11 @@
       <c r="D115" s="2" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E115">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>44</v>
       </c>
@@ -2686,8 +3034,11 @@
       <c r="D116" s="2" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E116">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>44</v>
       </c>
@@ -2700,8 +3051,11 @@
       <c r="D117" s="2" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E117">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>44</v>
       </c>
@@ -2714,8 +3068,11 @@
       <c r="D118" s="2" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E118">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>44</v>
       </c>
@@ -2728,8 +3085,11 @@
       <c r="D119" s="2" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E119">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>44</v>
       </c>
@@ -2742,8 +3102,11 @@
       <c r="D120" s="2" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E120">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>44</v>
       </c>
@@ -2756,8 +3119,11 @@
       <c r="D121" s="2" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E121">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>44</v>
       </c>
@@ -2770,8 +3136,11 @@
       <c r="D122" s="2" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E122">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>44</v>
       </c>
@@ -2784,8 +3153,11 @@
       <c r="D123" s="2" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E123">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>44</v>
       </c>
@@ -2798,8 +3170,11 @@
       <c r="D124" s="2" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E124">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>65</v>
       </c>
@@ -2812,8 +3187,11 @@
       <c r="D125" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E125">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>65</v>
       </c>
@@ -2826,8 +3204,11 @@
       <c r="D126" s="2" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E126">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>65</v>
       </c>
@@ -2840,8 +3221,11 @@
       <c r="D127" s="2" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E127">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>65</v>
       </c>
@@ -2854,8 +3238,11 @@
       <c r="D128" s="2" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E128">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>65</v>
       </c>
@@ -2868,8 +3255,11 @@
       <c r="D129" s="2" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E129">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>65</v>
       </c>
@@ -2882,8 +3272,11 @@
       <c r="D130" s="2" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E130">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>4</v>
       </c>
@@ -2896,8 +3289,11 @@
       <c r="D131" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E131">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>4</v>
       </c>
@@ -2910,8 +3306,11 @@
       <c r="D132" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E132">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>4</v>
       </c>
@@ -2924,8 +3323,11 @@
       <c r="D133" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E133">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>4</v>
       </c>
@@ -2938,8 +3340,11 @@
       <c r="D134" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E134">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>4</v>
       </c>
@@ -2952,8 +3357,11 @@
       <c r="D135" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E135">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>4</v>
       </c>
@@ -2966,8 +3374,11 @@
       <c r="D136" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E136">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>4</v>
       </c>
@@ -2980,8 +3391,11 @@
       <c r="D137" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E137">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>4</v>
       </c>
@@ -2994,8 +3408,11 @@
       <c r="D138" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E138">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>4</v>
       </c>
@@ -3008,8 +3425,11 @@
       <c r="D139" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E139">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>4</v>
       </c>
@@ -3022,8 +3442,11 @@
       <c r="D140" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E140">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>4</v>
       </c>
@@ -3036,8 +3459,11 @@
       <c r="D141" s="2" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E141">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>4</v>
       </c>
@@ -3050,8 +3476,11 @@
       <c r="D142" s="2" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E142">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>4</v>
       </c>
@@ -3064,8 +3493,11 @@
       <c r="D143" s="2" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E143">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>4</v>
       </c>
@@ -3078,8 +3510,11 @@
       <c r="D144" s="2" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E144">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>4</v>
       </c>
@@ -3092,8 +3527,11 @@
       <c r="D145" s="2" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E145">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>4</v>
       </c>
@@ -3106,8 +3544,11 @@
       <c r="D146" s="2" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E146">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>4</v>
       </c>
@@ -3120,8 +3561,11 @@
       <c r="D147" s="2" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E147">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>4</v>
       </c>
@@ -3134,8 +3578,11 @@
       <c r="D148" s="2" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E148">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>4</v>
       </c>
@@ -3148,8 +3595,11 @@
       <c r="D149" s="2" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E149">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>4</v>
       </c>
@@ -3162,8 +3612,11 @@
       <c r="D150" s="2" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E150">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>4</v>
       </c>
@@ -3176,8 +3629,11 @@
       <c r="D151" s="2" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E151">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>4</v>
       </c>
@@ -3190,8 +3646,11 @@
       <c r="D152" s="2" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E152">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>4</v>
       </c>
@@ -3204,8 +3663,11 @@
       <c r="D153" s="2" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E153">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>4</v>
       </c>
@@ -3218,8 +3680,11 @@
       <c r="D154" s="2" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E154">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>4</v>
       </c>
@@ -3232,8 +3697,11 @@
       <c r="D155" s="2" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E155">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>4</v>
       </c>
@@ -3246,8 +3714,11 @@
       <c r="D156" s="2" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E156">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>4</v>
       </c>
@@ -3260,8 +3731,11 @@
       <c r="D157" s="2" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E157">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>4</v>
       </c>
@@ -3274,8 +3748,11 @@
       <c r="D158" s="2" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E158">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>4</v>
       </c>
@@ -3288,8 +3765,11 @@
       <c r="D159" s="2" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E159">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>4</v>
       </c>
@@ -3301,6 +3781,9 @@
       </c>
       <c r="D160" s="2" t="s">
         <v>152</v>
+      </c>
+      <c r="E160">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>